<commit_message>
fix: username -> user_name
</commit_message>
<xml_diff>
--- a/03.バック設計/CODA_INOUT定義.xlsx
+++ b/03.バック設計/CODA_INOUT定義.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kakuda/iret/labo/CODA/CODA_DOCUMENT/03.バック設計/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7976ABD2-30F7-FF49-9483-5910473E1958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D72CC92-BCD2-614B-A1F9-04CC39202657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35080" yWindow="1760" windowWidth="27020" windowHeight="12240" activeTab="3" xr2:uid="{559C992E-6E4A-0D46-BDB3-6EB8904BAF6D}"/>
+    <workbookView xWindow="32140" yWindow="5260" windowWidth="27020" windowHeight="12240" activeTab="1" xr2:uid="{559C992E-6E4A-0D46-BDB3-6EB8904BAF6D}"/>
   </bookViews>
   <sheets>
     <sheet name="C001.ユーザーアカウント新規登録" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="66">
   <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
@@ -335,10 +335,6 @@
   </si>
   <si>
     <t>user_account_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>username</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1143,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC08D87-797A-DE4F-9F57-701A2FDC2220}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1247,7 +1243,7 @@
     <row r="9" spans="1:6">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -1288,7 +1284,7 @@
     <row r="13" spans="1:6">
       <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>36</v>
@@ -1374,7 +1370,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -1434,7 +1430,7 @@
     <row r="9" spans="1:6">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -1492,7 +1488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9D74D3-1BE5-6B49-A50E-82AD538A7883}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
@@ -1522,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1534,7 +1532,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -1558,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
@@ -1594,7 +1592,7 @@
     <row r="9" spans="1:6">
       <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>36</v>
@@ -1642,10 +1640,10 @@
     <row r="14" spans="1:6">
       <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>39</v>
@@ -1673,7 +1671,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1692,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -1777,7 +1775,7 @@
     <row r="9" spans="1:10">
       <c r="A9" s="14"/>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -1814,10 +1812,10 @@
     <row r="13" spans="1:10">
       <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
@@ -1826,10 +1824,10 @@
     <row r="14" spans="1:10">
       <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
@@ -1874,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -1959,10 +1957,10 @@
     <row r="9" spans="1:10">
       <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>39</v>
@@ -1976,10 +1974,10 @@
     <row r="10" spans="1:10">
       <c r="A10" s="14"/>
       <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>39</v>
@@ -2013,10 +2011,10 @@
     <row r="14" spans="1:10">
       <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
@@ -2061,7 +2059,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -2146,10 +2144,10 @@
     <row r="9" spans="1:10">
       <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>39</v>

</xml_diff>